<commit_message>
Prime Lead reports and SMS buttons
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateLeadSearch.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateLeadSearch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9FABA89-604F-4F99-BBD2-31FE9F636A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542007A-4727-43E0-80CB-9D22A1AE72F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1095" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Batch Number</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Original Campaign</t>
+  </si>
+  <si>
+    <t>Lead Prime Status</t>
+  </si>
+  <si>
+    <t>Date of Lead Prime Status</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,7 +230,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,67 +519,70 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection sqref="A1:AA1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="11" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" customWidth="1"/>
-    <col min="19" max="19" width="32.7109375" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1"/>
-    <col min="21" max="21" width="18.140625" customWidth="1"/>
-    <col min="22" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.85546875" customWidth="1"/>
-    <col min="27" max="27" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="7" width="18.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="11" width="18.1796875" customWidth="1"/>
+    <col min="12" max="12" width="15.26953125" customWidth="1"/>
+    <col min="13" max="16" width="13.81640625" customWidth="1"/>
+    <col min="17" max="17" width="14.81640625" customWidth="1"/>
+    <col min="18" max="18" width="18.1796875" customWidth="1"/>
+    <col min="19" max="19" width="32.7265625" customWidth="1"/>
+    <col min="20" max="20" width="13.81640625" customWidth="1"/>
+    <col min="21" max="21" width="18.1796875" customWidth="1"/>
+    <col min="22" max="24" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.26953125" customWidth="1"/>
+    <col min="26" max="26" width="16.81640625" customWidth="1"/>
+    <col min="27" max="27" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:29" ht="26" x14ac:dyDescent="0.6">
+      <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
     </row>
-    <row r="2" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:27" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:29" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -601,7 +609,7 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:27" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -628,8 +636,8 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:29" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -711,8 +719,14 @@
       <c r="AA6" s="11" t="s">
         <v>26</v>
       </c>
+      <c r="AB6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -739,11 +753,13 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="12"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>